<commit_message>
remove extra comma from Seattle, WA, zip
</commit_message>
<xml_diff>
--- a/GTEx Consortium Member List_September 2016_CT_updated.format_cc.xlsx
+++ b/GTEx Consortium Member List_September 2016_CT_updated.format_cc.xlsx
@@ -1128,9 +1128,6 @@
     <t>Akey</t>
   </si>
   <si>
-    <t>Department of Genome Sciences, University of Washington, Seattle, WA, 98195</t>
-  </si>
-  <si>
     <t>Takunda</t>
   </si>
   <si>
@@ -1183,9 +1180,6 @@
   </si>
   <si>
     <t>Lin</t>
-  </si>
-  <si>
-    <t>Division of Cardiology, University of Washington, Seattle, WA, 98195</t>
   </si>
   <si>
     <t>Marian</t>
@@ -2048,6 +2042,12 @@
   </si>
   <si>
     <t>Diego</t>
+  </si>
+  <si>
+    <t>Department of Genome Sciences, University of Washington, Seattle, WA 98195</t>
+  </si>
+  <si>
+    <t>Division of Cardiology, University of Washington, Seattle, WA 98195</t>
   </si>
 </sst>
 </file>
@@ -2397,8 +2397,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2698,6 +2700,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2740,11 +2745,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2798,6 +2800,7 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2851,6 +2854,7 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3121,7 +3125,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3132,8 +3136,8 @@
   <dimension ref="A1:O233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="2" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F206" sqref="F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3148,14 +3152,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.25" customHeight="1">
-      <c r="A1" s="76" t="s">
-        <v>484</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="A1" s="77" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="27" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -3168,18 +3172,18 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -3198,7 +3202,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -3212,7 +3216,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>9</v>
@@ -3230,7 +3234,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -3246,7 +3250,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -3260,7 +3264,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -3276,7 +3280,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -3290,7 +3294,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -3306,7 +3310,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3322,7 +3326,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -3338,7 +3342,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>34</v>
@@ -3354,7 +3358,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>34</v>
@@ -3441,13 +3445,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" customHeight="1">
       <c r="A20" s="21" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>6</v>
@@ -3459,7 +3463,7 @@
     </row>
     <row r="21" spans="1:6" ht="17.25" customHeight="1">
       <c r="A21" s="67" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="53"/>
@@ -3512,7 +3516,7 @@
         <v>74</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -3561,7 +3565,7 @@
         <v>86</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>90</v>
@@ -3721,7 +3725,7 @@
         <v>86</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>90</v>
@@ -3748,7 +3752,7 @@
         <v>86</v>
       </c>
       <c r="E38" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>90</v>
@@ -3766,7 +3770,7 @@
         <v>86</v>
       </c>
       <c r="E39" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>90</v>
@@ -3793,7 +3797,7 @@
         <v>86</v>
       </c>
       <c r="E40" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>90</v>
@@ -3811,7 +3815,7 @@
         <v>86</v>
       </c>
       <c r="E41" s="64" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>90</v>
@@ -3860,7 +3864,7 @@
         <v>144</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>145</v>
@@ -3887,13 +3891,13 @@
         <v>150</v>
       </c>
       <c r="D44" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>145</v>
       </c>
       <c r="F44" s="66" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -3914,7 +3918,7 @@
         <v>152</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>153</v>
@@ -3931,15 +3935,15 @@
       <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:15" ht="35.5" customHeight="1">
-      <c r="A46" s="85" t="s">
-        <v>537</v>
+      <c r="A46" s="71" t="s">
+        <v>535</v>
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="14" t="s">
         <v>156</v>
       </c>
       <c r="D46" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>145</v>
@@ -3955,7 +3959,7 @@
         <v>158</v>
       </c>
       <c r="D47" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>145</v>
@@ -3971,7 +3975,7 @@
         <v>160</v>
       </c>
       <c r="D48" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>145</v>
@@ -3987,7 +3991,7 @@
         <v>164</v>
       </c>
       <c r="D49" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E49" s="22" t="s">
         <v>145</v>
@@ -4003,7 +4007,7 @@
         <v>168</v>
       </c>
       <c r="D50" s="66" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>145</v>
@@ -4158,7 +4162,7 @@
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>176</v>
@@ -4296,7 +4300,7 @@
         <v>222</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>225</v>
@@ -4314,7 +4318,7 @@
         <v>227</v>
       </c>
       <c r="D67" s="66" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>228</v>
@@ -4332,7 +4336,7 @@
         <v>232</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="14"/>
@@ -4346,7 +4350,7 @@
         <v>234</v>
       </c>
       <c r="D69" s="66" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -4488,7 +4492,7 @@
         <v>274</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E78" s="14"/>
       <c r="F78" s="14"/>
@@ -4718,11 +4722,11 @@
     </row>
     <row r="90" spans="1:15" s="12" customFormat="1" ht="35" customHeight="1">
       <c r="A90" s="21" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B90" s="13"/>
       <c r="C90" s="13" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D90" s="13" t="s">
         <v>325</v>
@@ -4786,11 +4790,11 @@
       <c r="O92" s="11"/>
     </row>
     <row r="93" spans="1:15" s="12" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A93" s="71" t="s">
-        <v>533</v>
-      </c>
-      <c r="B93" s="72"/>
-      <c r="C93" s="72"/>
+      <c r="A93" s="72" t="s">
+        <v>531</v>
+      </c>
+      <c r="B93" s="73"/>
+      <c r="C93" s="73"/>
       <c r="D93" s="29"/>
       <c r="E93" s="29"/>
       <c r="F93" s="29"/>
@@ -4815,7 +4819,7 @@
         <v>347</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
@@ -4910,8 +4914,8 @@
       <c r="C98" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="D98" s="13" t="s">
-        <v>368</v>
+      <c r="D98" s="62" t="s">
+        <v>536</v>
       </c>
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
@@ -4934,7 +4938,7 @@
         <v>38</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E99" s="13" t="s">
         <v>6</v>
@@ -4952,14 +4956,14 @@
     </row>
     <row r="100" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A100" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E100" s="13"/>
       <c r="F100" s="13"/>
@@ -4979,10 +4983,10 @@
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
@@ -4998,14 +5002,14 @@
     </row>
     <row r="102" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A102" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B102" s="13"/>
       <c r="C102" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
@@ -5021,14 +5025,14 @@
     </row>
     <row r="103" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A103" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B103" s="13"/>
       <c r="C103" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
@@ -5044,17 +5048,17 @@
     </row>
     <row r="104" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A104" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B104" s="13"/>
       <c r="C104" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="E104" s="13" t="s">
-        <v>387</v>
+        <v>371</v>
+      </c>
+      <c r="E104" s="62" t="s">
+        <v>537</v>
       </c>
       <c r="F104" s="13"/>
       <c r="G104" s="11"/>
@@ -5078,7 +5082,7 @@
         <v>252</v>
       </c>
       <c r="D105" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
@@ -5094,14 +5098,14 @@
     </row>
     <row r="106" spans="1:15" s="12" customFormat="1" ht="36">
       <c r="A106" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B106" s="13"/>
       <c r="C106" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D106" s="46" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
@@ -5117,14 +5121,14 @@
     </row>
     <row r="107" spans="1:15" s="12" customFormat="1" ht="36">
       <c r="A107" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B107" s="13"/>
       <c r="C107" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D107" s="46" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E107" s="13"/>
       <c r="F107" s="13"/>
@@ -5144,10 +5148,10 @@
       </c>
       <c r="B108" s="22"/>
       <c r="C108" s="22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D108" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
@@ -5163,14 +5167,14 @@
     </row>
     <row r="109" spans="1:15" s="12" customFormat="1" ht="42.5" customHeight="1">
       <c r="A109" s="23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B109" s="22"/>
       <c r="C109" s="22" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D109" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
@@ -5186,14 +5190,14 @@
     </row>
     <row r="110" spans="1:15" s="12" customFormat="1" ht="42.5" customHeight="1">
       <c r="A110" s="21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B110" s="13"/>
       <c r="C110" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D110" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
@@ -5213,10 +5217,10 @@
       </c>
       <c r="B111" s="13"/>
       <c r="C111" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D111" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
@@ -5232,14 +5236,14 @@
     </row>
     <row r="112" spans="1:15" s="12" customFormat="1" ht="44.5" customHeight="1">
       <c r="A112" s="21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B112" s="13"/>
       <c r="C112" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D112" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
@@ -5255,14 +5259,14 @@
     </row>
     <row r="113" spans="1:15" s="12" customFormat="1" ht="27.5" customHeight="1">
       <c r="A113" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B113" s="13"/>
       <c r="C113" s="13" t="s">
         <v>204</v>
       </c>
       <c r="D113" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
@@ -5278,14 +5282,14 @@
     </row>
     <row r="114" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A114" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B114" s="13"/>
       <c r="C114" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D114" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
@@ -5301,14 +5305,14 @@
     </row>
     <row r="115" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A115" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B115" s="13"/>
       <c r="C115" s="13" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D115" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
@@ -5324,14 +5328,14 @@
     </row>
     <row r="116" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A116" s="21" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B116" s="13"/>
       <c r="C116" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D116" s="62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
@@ -5347,16 +5351,16 @@
     </row>
     <row r="117" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A117" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B117" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D117" s="62" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="13"/>
@@ -5372,14 +5376,14 @@
     </row>
     <row r="118" spans="1:15" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A118" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B118" s="13"/>
       <c r="C118" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D118" s="62" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
@@ -5395,16 +5399,16 @@
     </row>
     <row r="119" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A119" s="21" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D119" s="62" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
@@ -5420,49 +5424,49 @@
     </row>
     <row r="120" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A120" s="21" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B120" s="13"/>
       <c r="C120" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D120" s="62" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E120" s="13"/>
       <c r="F120" s="13"/>
     </row>
     <row r="121" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A121" s="21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D121" s="62" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
     </row>
     <row r="122" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A122" s="21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B122" s="13"/>
       <c r="C122" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D122" s="62" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
     </row>
     <row r="123" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A123" s="21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>59</v>
@@ -5510,41 +5514,41 @@
     </row>
     <row r="126" spans="1:15" s="12" customFormat="1" ht="42.5" customHeight="1">
       <c r="A126" s="21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B126" s="13"/>
       <c r="C126" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D126" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E126" s="13"/>
       <c r="F126" s="13"/>
     </row>
     <row r="127" spans="1:15" s="12" customFormat="1" ht="24">
       <c r="A127" s="21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B127" s="13"/>
       <c r="C127" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E127" s="13"/>
       <c r="F127" s="13"/>
     </row>
     <row r="128" spans="1:15" s="12" customFormat="1" ht="12">
-      <c r="A128" s="82" t="s">
-        <v>518</v>
-      </c>
-      <c r="B128" s="83"/>
-      <c r="C128" s="83"/>
-      <c r="D128" s="83"/>
-      <c r="E128" s="83"/>
-      <c r="F128" s="84"/>
+      <c r="A128" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="B128" s="84"/>
+      <c r="C128" s="84"/>
+      <c r="D128" s="84"/>
+      <c r="E128" s="84"/>
+      <c r="F128" s="85"/>
     </row>
     <row r="129" spans="1:6" s="12" customFormat="1" ht="36">
       <c r="A129" s="44" t="s">
@@ -5557,17 +5561,17 @@
         <v>18</v>
       </c>
       <c r="D129" s="59" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E129" s="44"/>
       <c r="F129" s="14"/>
     </row>
     <row r="130" spans="1:6" s="12" customFormat="1" ht="12">
-      <c r="A130" s="73" t="s">
-        <v>519</v>
-      </c>
-      <c r="B130" s="74"/>
-      <c r="C130" s="75"/>
+      <c r="A130" s="74" t="s">
+        <v>517</v>
+      </c>
+      <c r="B130" s="75"/>
+      <c r="C130" s="76"/>
       <c r="D130" s="32"/>
       <c r="E130" s="35"/>
       <c r="F130" s="32"/>
@@ -5583,7 +5587,7 @@
         <v>41</v>
       </c>
       <c r="D131" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E131" s="46"/>
       <c r="F131" s="43"/>
@@ -5597,7 +5601,7 @@
         <v>47</v>
       </c>
       <c r="D132" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E132" s="46"/>
       <c r="F132" s="43"/>
@@ -5611,7 +5615,7 @@
         <v>57</v>
       </c>
       <c r="D133" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E133" s="46"/>
       <c r="F133" s="43"/>
@@ -5627,7 +5631,7 @@
         <v>60</v>
       </c>
       <c r="D134" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E134" s="46"/>
       <c r="F134" s="43"/>
@@ -5643,7 +5647,7 @@
         <v>63</v>
       </c>
       <c r="D135" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E135" s="46"/>
       <c r="F135" s="43"/>
@@ -5665,11 +5669,11 @@
       <c r="F136" s="43"/>
     </row>
     <row r="137" spans="1:6" ht="12">
-      <c r="A137" s="73" t="s">
-        <v>520</v>
-      </c>
-      <c r="B137" s="74"/>
-      <c r="C137" s="75"/>
+      <c r="A137" s="74" t="s">
+        <v>518</v>
+      </c>
+      <c r="B137" s="75"/>
+      <c r="C137" s="76"/>
       <c r="D137" s="32"/>
       <c r="E137" s="29"/>
       <c r="F137" s="32"/>
@@ -5683,7 +5687,7 @@
         <v>83</v>
       </c>
       <c r="D138" s="60" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E138" s="46"/>
       <c r="F138" s="43"/>
@@ -5699,7 +5703,7 @@
         <v>89</v>
       </c>
       <c r="D139" s="60" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E139" s="46"/>
       <c r="F139" s="43"/>
@@ -5715,7 +5719,7 @@
         <v>95</v>
       </c>
       <c r="D140" s="60" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E140" s="46"/>
       <c r="F140" s="43"/>
@@ -5731,17 +5735,17 @@
         <v>102</v>
       </c>
       <c r="D141" s="60" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E141" s="46"/>
       <c r="F141" s="43"/>
     </row>
     <row r="142" spans="1:6" ht="54.5" customHeight="1">
-      <c r="A142" s="73" t="s">
-        <v>521</v>
-      </c>
-      <c r="B142" s="74"/>
-      <c r="C142" s="75"/>
+      <c r="A142" s="74" t="s">
+        <v>519</v>
+      </c>
+      <c r="B142" s="75"/>
+      <c r="C142" s="76"/>
       <c r="D142" s="32"/>
       <c r="E142" s="29"/>
       <c r="F142" s="32"/>
@@ -5757,7 +5761,7 @@
         <v>112</v>
       </c>
       <c r="D143" s="60" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E143" s="46"/>
       <c r="F143" s="43"/>
@@ -5773,24 +5777,24 @@
         <v>122</v>
       </c>
       <c r="D144" s="60" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E144" s="46"/>
       <c r="F144" s="43"/>
     </row>
     <row r="145" spans="1:6" ht="50.5" customHeight="1">
-      <c r="A145" s="80" t="s">
-        <v>522</v>
-      </c>
-      <c r="B145" s="81"/>
-      <c r="C145" s="81"/>
+      <c r="A145" s="81" t="s">
+        <v>520</v>
+      </c>
+      <c r="B145" s="82"/>
+      <c r="C145" s="82"/>
       <c r="D145" s="35"/>
       <c r="E145" s="45"/>
       <c r="F145" s="32"/>
     </row>
     <row r="146" spans="1:6" ht="29" customHeight="1">
       <c r="A146" s="64" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>127</v>
@@ -5799,14 +5803,14 @@
         <v>128</v>
       </c>
       <c r="D146" s="65" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E146" s="12"/>
       <c r="F146" s="14"/>
     </row>
     <row r="147" spans="1:6" ht="28.25" customHeight="1">
       <c r="A147" s="68" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B147" s="33"/>
       <c r="C147" s="34"/>
@@ -5825,7 +5829,7 @@
         <v>140</v>
       </c>
       <c r="D148" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E148" s="46"/>
       <c r="F148" s="47"/>
@@ -5841,7 +5845,7 @@
         <v>149</v>
       </c>
       <c r="D149" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E149" s="46"/>
       <c r="F149" s="47"/>
@@ -5855,7 +5859,7 @@
         <v>155</v>
       </c>
       <c r="D150" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E150" s="46"/>
       <c r="F150" s="47"/>
@@ -5869,7 +5873,7 @@
         <v>162</v>
       </c>
       <c r="D151" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E151" s="46"/>
       <c r="F151" s="47"/>
@@ -5883,7 +5887,7 @@
         <v>167</v>
       </c>
       <c r="D152" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E152" s="46"/>
       <c r="F152" s="47"/>
@@ -5897,7 +5901,7 @@
         <v>173</v>
       </c>
       <c r="D153" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E153" s="46"/>
       <c r="F153" s="47"/>
@@ -5913,7 +5917,7 @@
         <v>182</v>
       </c>
       <c r="D154" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E154" s="46"/>
       <c r="F154" s="47"/>
@@ -5927,7 +5931,7 @@
         <v>188</v>
       </c>
       <c r="D155" s="63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E155" s="46"/>
       <c r="F155" s="47"/>
@@ -5941,7 +5945,7 @@
         <v>196</v>
       </c>
       <c r="D156" s="63" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E156" s="46"/>
       <c r="F156" s="47"/>
@@ -5955,7 +5959,7 @@
         <v>200</v>
       </c>
       <c r="D157" s="63" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E157" s="46"/>
       <c r="F157" s="47"/>
@@ -5969,7 +5973,7 @@
         <v>204</v>
       </c>
       <c r="D158" s="63" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E158" s="46"/>
       <c r="F158" s="47"/>
@@ -5983,7 +5987,7 @@
         <v>208</v>
       </c>
       <c r="D159" s="63" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E159" s="46"/>
       <c r="F159" s="47"/>
@@ -5999,7 +6003,7 @@
         <v>215</v>
       </c>
       <c r="D160" s="63" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E160" s="46"/>
       <c r="F160" s="47"/>
@@ -6013,7 +6017,7 @@
         <v>220</v>
       </c>
       <c r="D161" s="63" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E161" s="46"/>
       <c r="F161" s="47"/>
@@ -6027,7 +6031,7 @@
         <v>224</v>
       </c>
       <c r="D162" s="63" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E162" s="46"/>
       <c r="F162" s="47"/>
@@ -6041,7 +6045,7 @@
         <v>233</v>
       </c>
       <c r="D163" s="63" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E163" s="46"/>
       <c r="F163" s="47"/>
@@ -6055,7 +6059,7 @@
         <v>236</v>
       </c>
       <c r="D164" s="63" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E164" s="46"/>
       <c r="F164" s="47"/>
@@ -6069,14 +6073,14 @@
         <v>242</v>
       </c>
       <c r="D165" s="63" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E165" s="46"/>
       <c r="F165" s="47"/>
     </row>
     <row r="166" spans="1:6" ht="27.5" customHeight="1">
       <c r="A166" s="68" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B166" s="33"/>
       <c r="C166" s="34"/>
@@ -6095,7 +6099,7 @@
         <v>253</v>
       </c>
       <c r="D167" s="60" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E167" s="46"/>
       <c r="F167" s="43"/>
@@ -6111,7 +6115,7 @@
         <v>254</v>
       </c>
       <c r="D168" s="60" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E168" s="46"/>
       <c r="F168" s="43"/>
@@ -6125,7 +6129,7 @@
         <v>257</v>
       </c>
       <c r="D169" s="60" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E169" s="46"/>
       <c r="F169" s="43"/>
@@ -6141,7 +6145,7 @@
         <v>261</v>
       </c>
       <c r="D170" s="60" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E170" s="46"/>
       <c r="F170" s="43"/>
@@ -6155,7 +6159,7 @@
         <v>266</v>
       </c>
       <c r="D171" s="60" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E171" s="46"/>
       <c r="F171" s="43"/>
@@ -6189,11 +6193,11 @@
       <c r="F173" s="43"/>
     </row>
     <row r="174" spans="1:6" ht="12">
-      <c r="A174" s="73" t="s">
-        <v>525</v>
-      </c>
-      <c r="B174" s="74"/>
-      <c r="C174" s="75"/>
+      <c r="A174" s="74" t="s">
+        <v>523</v>
+      </c>
+      <c r="B174" s="75"/>
+      <c r="C174" s="76"/>
       <c r="D174" s="32"/>
       <c r="E174" s="29"/>
       <c r="F174" s="32"/>
@@ -6209,7 +6213,7 @@
         <v>283</v>
       </c>
       <c r="D175" s="60" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E175" s="46"/>
       <c r="F175" s="43"/>
@@ -6225,7 +6229,7 @@
         <v>292</v>
       </c>
       <c r="D176" s="60" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E176" s="46"/>
       <c r="F176" s="43"/>
@@ -6239,7 +6243,7 @@
         <v>296</v>
       </c>
       <c r="D177" s="60" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E177" s="46"/>
       <c r="F177" s="43"/>
@@ -6255,17 +6259,17 @@
         <v>301</v>
       </c>
       <c r="D178" s="60" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E178" s="46"/>
       <c r="F178" s="43"/>
     </row>
     <row r="179" spans="1:6" ht="13.25" customHeight="1">
-      <c r="A179" s="73" t="s">
-        <v>526</v>
-      </c>
-      <c r="B179" s="74"/>
-      <c r="C179" s="75"/>
+      <c r="A179" s="74" t="s">
+        <v>524</v>
+      </c>
+      <c r="B179" s="75"/>
+      <c r="C179" s="76"/>
       <c r="D179" s="32"/>
       <c r="E179" s="29"/>
       <c r="F179" s="32"/>
@@ -6281,7 +6285,7 @@
         <v>304</v>
       </c>
       <c r="D180" s="60" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E180" s="46"/>
       <c r="F180" s="43"/>
@@ -6297,17 +6301,17 @@
         <v>184</v>
       </c>
       <c r="D181" s="60" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E181" s="46"/>
       <c r="F181" s="43"/>
     </row>
     <row r="182" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A182" s="73" t="s">
-        <v>527</v>
-      </c>
-      <c r="B182" s="74"/>
-      <c r="C182" s="75"/>
+      <c r="A182" s="74" t="s">
+        <v>525</v>
+      </c>
+      <c r="B182" s="75"/>
+      <c r="C182" s="76"/>
       <c r="D182" s="32"/>
       <c r="E182" s="29"/>
       <c r="F182" s="32"/>
@@ -6540,11 +6544,11 @@
     </row>
     <row r="198" spans="1:6" ht="12">
       <c r="A198" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B198" s="19"/>
       <c r="C198" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D198" s="56" t="s">
         <v>339</v>
@@ -6554,13 +6558,13 @@
     </row>
     <row r="199" spans="1:6" ht="12">
       <c r="A199" s="13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B199" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D199" s="13" t="s">
         <v>339</v>
@@ -6569,80 +6573,80 @@
       <c r="F199" s="13"/>
     </row>
     <row r="200" spans="1:6" ht="12">
-      <c r="A200" s="77" t="s">
-        <v>528</v>
-      </c>
-      <c r="B200" s="78"/>
-      <c r="C200" s="79"/>
+      <c r="A200" s="78" t="s">
+        <v>526</v>
+      </c>
+      <c r="B200" s="79"/>
+      <c r="C200" s="80"/>
       <c r="D200" s="29"/>
       <c r="E200" s="29"/>
       <c r="F200" s="45"/>
     </row>
     <row r="201" spans="1:6" ht="12">
       <c r="A201" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B201" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C201" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D201" s="61" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E201" s="46"/>
       <c r="F201" s="43"/>
     </row>
     <row r="202" spans="1:6" ht="24">
       <c r="A202" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B202" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C202" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="D202" s="42" t="s">
         <v>379</v>
-      </c>
-      <c r="D202" s="42" t="s">
-        <v>380</v>
       </c>
       <c r="E202" s="46"/>
       <c r="F202" s="43"/>
     </row>
     <row r="203" spans="1:6" ht="12.75" customHeight="1">
       <c r="A203" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B203" s="14"/>
       <c r="C203" s="36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D203" s="41" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E203" s="46"/>
       <c r="F203" s="43"/>
     </row>
     <row r="204" spans="1:6" ht="32" customHeight="1">
       <c r="A204" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B204" s="14" t="s">
         <v>186</v>
       </c>
       <c r="C204" s="36" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D204" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E204" s="46"/>
       <c r="F204" s="43"/>
     </row>
     <row r="205" spans="1:6" ht="29.5" customHeight="1">
       <c r="A205" s="68" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B205" s="33"/>
       <c r="C205" s="34"/>
@@ -6652,16 +6656,16 @@
     </row>
     <row r="206" spans="1:6" ht="29" customHeight="1">
       <c r="A206" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B206" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D206" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E206" s="46"/>
       <c r="F206" s="43"/>
@@ -6672,38 +6676,38 @@
       </c>
       <c r="B207" s="14"/>
       <c r="C207" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D207" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E207" s="46"/>
       <c r="F207" s="43"/>
     </row>
     <row r="208" spans="1:6" ht="30" customHeight="1">
       <c r="A208" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B208" s="14"/>
       <c r="C208" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D208" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E208" s="46"/>
       <c r="F208" s="43"/>
     </row>
     <row r="209" spans="1:6" ht="27" customHeight="1">
       <c r="A209" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B209" s="14"/>
       <c r="C209" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E209" s="46"/>
       <c r="F209" s="43"/>
@@ -6714,45 +6718,45 @@
       </c>
       <c r="B210" s="14"/>
       <c r="C210" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D210" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E210" s="46"/>
       <c r="F210" s="43"/>
     </row>
     <row r="211" spans="1:6" ht="30" customHeight="1">
       <c r="A211" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B211" s="14"/>
       <c r="C211" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D211" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E211" s="46"/>
       <c r="F211" s="43"/>
     </row>
     <row r="212" spans="1:6" ht="29" customHeight="1">
       <c r="A212" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B212" s="14"/>
       <c r="C212" s="14" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D212" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E212" s="46"/>
       <c r="F212" s="43"/>
     </row>
     <row r="213" spans="1:6" ht="15.5" customHeight="1">
       <c r="A213" s="68" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B213" s="33"/>
       <c r="C213" s="34"/>
@@ -6762,44 +6766,44 @@
     </row>
     <row r="214" spans="1:6" ht="41.5" customHeight="1">
       <c r="A214" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B214" s="14"/>
       <c r="C214" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D214" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E214" s="46"/>
       <c r="F214" s="43"/>
     </row>
     <row r="215" spans="1:6" ht="43.25" customHeight="1">
       <c r="A215" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B215" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C215" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D215" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E215" s="46"/>
       <c r="F215" s="43"/>
     </row>
     <row r="216" spans="1:6" ht="35" customHeight="1">
       <c r="A216" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B216" s="14"/>
       <c r="C216" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D216" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E216" s="46"/>
       <c r="F216" s="43"/>
@@ -6812,24 +6816,24 @@
         <v>40</v>
       </c>
       <c r="C217" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D217" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E217" s="46"/>
       <c r="F217" s="43"/>
     </row>
     <row r="218" spans="1:6" ht="31.25" customHeight="1">
       <c r="A218" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B218" s="14"/>
       <c r="C218" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D218" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E218" s="46"/>
       <c r="F218" s="43"/>
@@ -6840,24 +6844,24 @@
       </c>
       <c r="B219" s="14"/>
       <c r="C219" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D219" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E219" s="46"/>
       <c r="F219" s="43"/>
     </row>
     <row r="220" spans="1:6" ht="32" customHeight="1">
       <c r="A220" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B220" s="14"/>
       <c r="C220" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D220" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E220" s="46"/>
       <c r="F220" s="43"/>
@@ -6868,10 +6872,10 @@
       </c>
       <c r="B221" s="14"/>
       <c r="C221" s="14" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D221" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E221" s="46"/>
       <c r="F221" s="43"/>
@@ -6882,17 +6886,17 @@
       </c>
       <c r="B222" s="14"/>
       <c r="C222" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D222" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E222" s="46"/>
       <c r="F222" s="43"/>
     </row>
     <row r="223" spans="1:6" ht="12.75" customHeight="1">
       <c r="A223" s="68" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B223" s="8"/>
       <c r="C223" s="9"/>
@@ -6902,33 +6906,33 @@
     </row>
     <row r="224" spans="1:6" ht="13.5" customHeight="1">
       <c r="A224" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B224" s="14"/>
       <c r="C224" s="36" t="s">
         <v>25</v>
       </c>
       <c r="D224" s="43" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E224" s="36"/>
       <c r="F224" s="37"/>
     </row>
     <row r="225" spans="1:15" s="12" customFormat="1" ht="36">
       <c r="A225" s="16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B225" s="14" t="s">
         <v>300</v>
       </c>
       <c r="C225" s="36" t="s">
+        <v>450</v>
+      </c>
+      <c r="D225" s="43" t="s">
+        <v>451</v>
+      </c>
+      <c r="E225" s="36" t="s">
         <v>452</v>
-      </c>
-      <c r="D225" s="43" t="s">
-        <v>453</v>
-      </c>
-      <c r="E225" s="36" t="s">
-        <v>454</v>
       </c>
       <c r="F225" s="37"/>
       <c r="G225" s="11"/>
@@ -6943,17 +6947,17 @@
     </row>
     <row r="226" spans="1:15" s="12" customFormat="1" ht="31.25" customHeight="1">
       <c r="A226" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B226" s="15"/>
       <c r="C226" s="38" t="s">
+        <v>454</v>
+      </c>
+      <c r="D226" s="49" t="s">
+        <v>455</v>
+      </c>
+      <c r="E226" s="38" t="s">
         <v>456</v>
-      </c>
-      <c r="D226" s="49" t="s">
-        <v>457</v>
-      </c>
-      <c r="E226" s="38" t="s">
-        <v>458</v>
       </c>
       <c r="F226" s="37"/>
       <c r="G226" s="11"/>
@@ -6974,10 +6978,10 @@
         <v>11</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D227" s="24" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E227" s="38"/>
       <c r="F227" s="37"/>
@@ -6993,14 +6997,14 @@
     </row>
     <row r="228" spans="1:15" s="12" customFormat="1" ht="42.5" customHeight="1">
       <c r="A228" s="15" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B228" s="15"/>
       <c r="C228" s="38" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D228" s="49" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E228" s="38"/>
       <c r="F228" s="37"/>
@@ -7016,14 +7020,14 @@
     </row>
     <row r="229" spans="1:15" s="12" customFormat="1" ht="30.5" customHeight="1">
       <c r="A229" s="15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B229" s="15"/>
       <c r="C229" s="38" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D229" s="49" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E229" s="38"/>
       <c r="F229" s="37"/>
@@ -7039,16 +7043,16 @@
     </row>
     <row r="230" spans="1:15" s="12" customFormat="1" ht="28.5" customHeight="1">
       <c r="A230" s="15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B230" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C230" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D230" s="49" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E230" s="38"/>
       <c r="F230" s="37"/>
@@ -7064,14 +7068,14 @@
     </row>
     <row r="231" spans="1:15" s="12" customFormat="1" ht="32" customHeight="1">
       <c r="A231" s="15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B231" s="15"/>
       <c r="C231" s="38" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D231" s="49" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E231" s="38"/>
       <c r="F231" s="37"/>
@@ -7091,10 +7095,10 @@
       </c>
       <c r="B232" s="15"/>
       <c r="C232" s="38" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D232" s="49" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E232" s="38"/>
       <c r="F232" s="37"/>
@@ -7110,16 +7114,16 @@
     </row>
     <row r="233" spans="1:15" s="12" customFormat="1" ht="28.25" customHeight="1">
       <c r="A233" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B233" s="15" t="s">
         <v>59</v>
       </c>
       <c r="C233" s="38" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D233" s="49" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E233" s="38"/>
       <c r="F233" s="37"/>

</xml_diff>